<commit_message>
Updated vignette tables and figure caption format
</commit_message>
<xml_diff>
--- a/vignettes/data/asv_small.xlsx
+++ b/vignettes/data/asv_small.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Munkk\Desktop\Holomics\vignettes\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katha\AIT\Holomics\vignettes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56158B64-E2D0-48D2-92F2-FF71CBE46F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA7E002-6B18-491C-BFB2-5DE5AE86AD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -46,38 +46,44 @@
     <t>ASV_1101</t>
   </si>
   <si>
-    <t>V1_1_t0</t>
-  </si>
-  <si>
-    <t>V1_2_t0</t>
-  </si>
-  <si>
-    <t>V1_3_t0</t>
-  </si>
-  <si>
-    <t>V1_4_t0</t>
-  </si>
-  <si>
-    <t>V2_1_t0</t>
-  </si>
-  <si>
-    <t>V2_2_t0</t>
-  </si>
-  <si>
-    <t>V2_3_t0</t>
-  </si>
-  <si>
-    <t>V2_4_t0</t>
+    <t>Sample1</t>
+  </si>
+  <si>
+    <t>Sample2</t>
+  </si>
+  <si>
+    <t>Sample3</t>
+  </si>
+  <si>
+    <t>Sample4</t>
+  </si>
+  <si>
+    <t>Sample5</t>
+  </si>
+  <si>
+    <t>Sample6</t>
+  </si>
+  <si>
+    <t>Sample7</t>
+  </si>
+  <si>
+    <t>Sample8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -404,7 +410,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,6 +650,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>